<commit_message>
continue processing, extend analysis NB
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FCC6F2-6E4D-174C-9A4A-41FB7D1C0E18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9301A64-D96F-524B-B2D2-862D4C590534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8180" yWindow="25280" windowWidth="24940" windowHeight="14980" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
+    <workbookView xWindow="7060" yWindow="25020" windowWidth="24940" windowHeight="14980" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>coworking</t>
   </si>
@@ -42,9 +42,6 @@
     <t>degree centrality</t>
   </si>
   <si>
-    <t>normality</t>
-  </si>
-  <si>
     <t>ghosting</t>
   </si>
   <si>
@@ -73,6 +70,15 @@
   </si>
   <si>
     <t>man bun</t>
+  </si>
+  <si>
+    <t>climate emergency</t>
+  </si>
+  <si>
+    <t>sign</t>
+  </si>
+  <si>
+    <t>word of the year</t>
   </si>
 </sst>
 </file>
@@ -424,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEC375-6E1C-D542-ABA0-0194DB27DDCA}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,10 +446,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -462,7 +468,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -474,12 +480,12 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -491,12 +497,12 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -510,7 +516,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -524,7 +530,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -538,7 +544,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -552,7 +558,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -562,6 +568,23 @@
       </c>
       <c r="D9">
         <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
after HJS meeting, fixe error, continue processing, introduce filters for NB analyses
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9301A64-D96F-524B-B2D2-862D4C590534}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7500232A-9B5F-EE4A-A55B-D950E7E36FD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="25020" windowWidth="24940" windowHeight="14980" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add proper files (again)
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7500232A-9B5F-EE4A-A55B-D950E7E36FD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA66AF-7E0B-ED40-83D4-EA2C493D6F2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="25020" windowWidth="24940" windowHeight="14980" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
+    <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>coworking</t>
   </si>
@@ -39,9 +39,6 @@
     <t>S-curve</t>
   </si>
   <si>
-    <t>degree centrality</t>
-  </si>
-  <si>
     <t>ghosting</t>
   </si>
   <si>
@@ -79,6 +76,21 @@
   </si>
   <si>
     <t>word of the year</t>
+  </si>
+  <si>
+    <t>climate crisis</t>
+  </si>
+  <si>
+    <t>refugee crisis</t>
+  </si>
+  <si>
+    <t>cent_total</t>
+  </si>
+  <si>
+    <t>cent_diac</t>
+  </si>
+  <si>
+    <t>blockchain</t>
   </si>
 </sst>
 </file>
@@ -430,29 +442,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEC375-6E1C-D542-ABA0-0194DB27DDCA}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -462,13 +477,13 @@
       <c r="C2">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -476,16 +491,16 @@
       <c r="C3">
         <v>5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -493,16 +508,16 @@
       <c r="C4">
         <v>5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -510,13 +525,13 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -524,13 +539,13 @@
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -538,13 +553,13 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -552,13 +567,13 @@
       <c r="C8">
         <v>5</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -566,13 +581,13 @@
       <c r="C9">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>5</v>
@@ -580,11 +595,47 @@
       <c r="C10">
         <v>3</v>
       </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>15</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up diff_start; remove handle uses; process again
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247DCCDE-07BC-1F41-9C9C-C541EB69D31E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3364361F-CE1E-4E4D-BCC9-3089BBB61148}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6400" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>coworking</t>
   </si>
@@ -123,15 +123,38 @@
     <t>cent high</t>
   </si>
   <si>
-    <t>solpreneur</t>
+    <t>deep learning</t>
+  </si>
+  <si>
+    <t>solopreneur</t>
+  </si>
+  <si>
+    <t>upskill</t>
+  </si>
+  <si>
+    <t>deepfake</t>
+  </si>
+  <si>
+    <t>followership</t>
+  </si>
+  <si>
+    <t>Brexiter / Brexiteer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -159,8 +182,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -475,10 +499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEC375-6E1C-D542-ABA0-0194DB27DDCA}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,26 +511,26 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -791,10 +816,74 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B19">
-        <v>4</v>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add diff start setting to processing
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86CFDF72-7EB7-2B4E-8393-F81E3CFCD82B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814B03EA-F409-8645-9B1C-795DF37DD926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
@@ -240,27 +240,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1218,7 +1198,7 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="A1:I1048576">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$I1=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
re-pick test cases; refine plots
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2554FA-5590-5E42-B891-9997388E325A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1B14A0-CC38-F54E-BCB6-A4A7D7067A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="evaluation" sheetId="1" r:id="rId1"/>
+    <sheet name="selection" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$I$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">evaluation!$A$1:$I$31</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>coworking</t>
   </si>
@@ -178,6 +179,75 @@
   </si>
   <si>
     <t>cent_diac: constantly low</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>stability</t>
+  </si>
+  <si>
+    <t>stable</t>
+  </si>
+  <si>
+    <t>topical</t>
+  </si>
+  <si>
+    <t>poppygate</t>
+  </si>
+  <si>
+    <t>trend</t>
+  </si>
+  <si>
+    <t>decreasing</t>
+  </si>
+  <si>
+    <t>time window</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>centralization</t>
+  </si>
+  <si>
+    <t>hyperlocal</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>alt-left</t>
+  </si>
+  <si>
+    <t>solopreneur, robo-signing</t>
+  </si>
+  <si>
+    <t>robo-signing</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>lemma</t>
+  </si>
+  <si>
+    <t>unstable</t>
+  </si>
+  <si>
+    <t>newsjacking</t>
   </si>
 </sst>
 </file>
@@ -566,7 +636,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1204,4 +1274,233 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8548A97-1726-DA44-988E-7F7E609BAEDB}">
+  <dimension ref="A1:P11"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="16" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7">
+        <v>2</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="7">
+        <v>1</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improve case study selection; add cum. freq. plots
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1B14A0-CC38-F54E-BCB6-A4A7D7067A76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3C90F-8EAB-3946-BE7C-29EF53D76F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
   <si>
     <t>coworking</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>newsjacking</t>
+  </si>
+  <si>
+    <t>circular economy</t>
+  </si>
+  <si>
+    <t>S-curve, a bit spikey</t>
+  </si>
+  <si>
+    <t>100 k</t>
   </si>
 </sst>
 </file>
@@ -632,11 +641,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEC375-6E1C-D542-ABA0-0194DB27DDCA}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,6 +1262,20 @@
       <c r="F31"/>
       <c r="G31"/>
       <c r="I31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I31" xr:uid="{5B8BAF05-1FD3-624C-9941-B290D0C9FED2}">

</xml_diff>

<commit_message>
switch from _birther_ to _poppygate_
</commit_message>
<xml_diff>
--- a/cases.xlsx
+++ b/cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quirin/promo/sna/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E3C90F-8EAB-3946-BE7C-29EF53D76F03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B2AC72-3E84-6547-A3E8-2780443DD115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="24460" windowWidth="25600" windowHeight="15540" xr2:uid="{A18AA071-A656-6944-AD38-1A9FC623F5B7}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="selection" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">evaluation!$A$1:$I$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">evaluation!$A$1:$J$31</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>coworking</t>
   </si>
@@ -256,7 +256,31 @@
     <t>S-curve, a bit spikey</t>
   </si>
   <si>
-    <t>100 k</t>
+    <t>burquini</t>
+  </si>
+  <si>
+    <t>Pizzagate</t>
+  </si>
+  <si>
+    <t>cherpumple</t>
+  </si>
+  <si>
+    <t>COEF_VAR</t>
+  </si>
+  <si>
+    <t>increasing, spikey</t>
+  </si>
+  <si>
+    <t>birther</t>
+  </si>
+  <si>
+    <t>deg_diac: low, decr; USES_TOT: very low</t>
+  </si>
+  <si>
+    <t>DEG_DIAC: decreasing</t>
+  </si>
+  <si>
+    <t>DEG_DIAC: low</t>
   </si>
 </sst>
 </file>
@@ -319,7 +343,27 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -641,21 +685,21 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FEEC375-6E1C-D542-ABA0-0194DB27DDCA}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="10.83203125" style="7"/>
-    <col min="9" max="9" width="10.83203125" style="7"/>
+    <col min="2" max="8" width="10.83203125" style="7"/>
+    <col min="10" max="10" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>36</v>
       </c>
@@ -666,25 +710,28 @@
         <v>35</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -694,22 +741,23 @@
       <c r="C2" s="6">
         <v>5</v>
       </c>
-      <c r="D2" s="6">
-        <v>5</v>
-      </c>
-      <c r="E2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6">
+        <v>5</v>
+      </c>
       <c r="F2" s="6"/>
-      <c r="G2" s="6">
-        <v>3</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="G2" s="6"/>
+      <c r="H2" s="6">
+        <v>3</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -717,7 +765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -726,30 +774,31 @@
       </c>
       <c r="C4"/>
       <c r="D4"/>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4"/>
-      <c r="G4">
-        <v>5</v>
-      </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="E4"/>
+      <c r="F4">
+        <v>5</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B5" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="7">
-        <v>3</v>
-      </c>
-      <c r="G5" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="H5" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -761,9 +810,10 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H6"/>
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -775,29 +825,30 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H7"/>
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="7">
-        <v>3</v>
-      </c>
       <c r="E8" s="7">
-        <v>5</v>
-      </c>
-      <c r="G8" s="7">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="H8" s="7">
+        <v>5</v>
+      </c>
+      <c r="I8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
@@ -807,20 +858,20 @@
       <c r="C9" s="7">
         <v>4</v>
       </c>
-      <c r="D9" s="7">
-        <v>3</v>
-      </c>
-      <c r="F9" s="7">
-        <v>1</v>
+      <c r="E9" s="7">
+        <v>3</v>
       </c>
       <c r="G9" s="7">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -830,20 +881,20 @@
       <c r="C10" s="7">
         <v>1</v>
       </c>
-      <c r="D10" s="7">
-        <v>3</v>
-      </c>
       <c r="E10" s="7">
         <v>3</v>
       </c>
-      <c r="G10" s="7">
-        <v>5</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="F10" s="7">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
+      <c r="I10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -853,37 +904,37 @@
       <c r="C11" s="7">
         <v>5</v>
       </c>
-      <c r="E11" s="7">
-        <v>5</v>
-      </c>
-      <c r="G11" s="7">
-        <v>5</v>
-      </c>
-      <c r="H11" s="2" t="s">
+      <c r="F11" s="7">
+        <v>5</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="I11" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="7">
         <v>3</v>
       </c>
-      <c r="D12" s="7">
-        <v>4</v>
-      </c>
       <c r="E12" s="7">
-        <v>3</v>
-      </c>
-      <c r="G12" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3</v>
+      </c>
+      <c r="H12" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -891,19 +942,20 @@
         <v>2</v>
       </c>
       <c r="C13"/>
-      <c r="D13">
-        <v>4</v>
-      </c>
+      <c r="D13"/>
       <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
         <v>2</v>
       </c>
-      <c r="F13"/>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="I13"/>
-    </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="G13"/>
+      <c r="H13">
+        <v>5</v>
+      </c>
+      <c r="J13"/>
+    </row>
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -911,36 +963,37 @@
         <v>1</v>
       </c>
       <c r="C14"/>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14"/>
+      <c r="D14"/>
+      <c r="E14">
+        <v>5</v>
+      </c>
       <c r="F14"/>
-      <c r="G14">
-        <v>3</v>
-      </c>
-      <c r="I14">
+      <c r="G14"/>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="J14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
       <c r="B15" s="7">
         <v>4</v>
       </c>
-      <c r="D15" s="7">
-        <v>4</v>
-      </c>
       <c r="E15" s="7">
+        <v>4</v>
+      </c>
+      <c r="F15" s="7">
         <v>2</v>
       </c>
-      <c r="G15" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -950,60 +1003,60 @@
       <c r="C16" s="7">
         <v>4</v>
       </c>
-      <c r="D16" s="7">
-        <v>5</v>
-      </c>
       <c r="E16" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F16" s="7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="7">
         <v>4</v>
       </c>
-      <c r="H16" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H16" s="7">
+        <v>4</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="7">
         <v>3</v>
       </c>
-      <c r="E17" s="7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F17" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="7">
         <v>4</v>
       </c>
-      <c r="D18" s="7">
-        <v>4</v>
-      </c>
       <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="7">
         <v>2</v>
       </c>
-      <c r="F18" s="7">
-        <v>4</v>
-      </c>
       <c r="G18" s="7">
         <v>4</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="7">
+        <v>4</v>
+      </c>
+      <c r="I18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -1013,17 +1066,17 @@
       <c r="C19" s="7">
         <v>3</v>
       </c>
-      <c r="E19" s="7">
-        <v>5</v>
-      </c>
-      <c r="G19" s="7">
-        <v>3</v>
-      </c>
-      <c r="I19" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="7">
+        <v>5</v>
+      </c>
+      <c r="H19" s="7">
+        <v>3</v>
+      </c>
+      <c r="J19" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1031,19 +1084,20 @@
         <v>2</v>
       </c>
       <c r="C20"/>
-      <c r="D20">
-        <v>5</v>
-      </c>
-      <c r="E20"/>
+      <c r="D20"/>
+      <c r="E20">
+        <v>5</v>
+      </c>
       <c r="F20"/>
-      <c r="G20">
-        <v>4</v>
-      </c>
-      <c r="I20">
+      <c r="G20"/>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="J20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1051,19 +1105,20 @@
         <v>1</v>
       </c>
       <c r="C21"/>
-      <c r="D21">
-        <v>5</v>
-      </c>
-      <c r="E21"/>
+      <c r="D21"/>
+      <c r="E21">
+        <v>5</v>
+      </c>
       <c r="F21"/>
-      <c r="G21">
-        <v>5</v>
-      </c>
-      <c r="I21">
+      <c r="G21"/>
+      <c r="H21">
+        <v>5</v>
+      </c>
+      <c r="J21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -1071,19 +1126,20 @@
         <v>1</v>
       </c>
       <c r="C22"/>
-      <c r="D22">
-        <v>5</v>
-      </c>
-      <c r="E22"/>
+      <c r="D22"/>
+      <c r="E22">
+        <v>5</v>
+      </c>
       <c r="F22"/>
-      <c r="G22">
-        <v>5</v>
-      </c>
-      <c r="I22">
+      <c r="G22"/>
+      <c r="H22">
+        <v>5</v>
+      </c>
+      <c r="J22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>18</v>
       </c>
@@ -1093,20 +1149,20 @@
       <c r="C23" s="7">
         <v>1</v>
       </c>
-      <c r="E23" s="7">
-        <v>5</v>
-      </c>
       <c r="F23" s="7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G23" s="7">
-        <v>4</v>
-      </c>
-      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="7">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -1118,32 +1174,33 @@
       <c r="E24"/>
       <c r="F24"/>
       <c r="G24"/>
-      <c r="I24"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H24"/>
+      <c r="J24"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="7">
         <v>5</v>
       </c>
-      <c r="D25" s="7">
-        <v>3</v>
-      </c>
       <c r="E25" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F25" s="7">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G25" s="7">
         <v>5</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="7">
+        <v>5</v>
+      </c>
+      <c r="I25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>26</v>
       </c>
@@ -1153,17 +1210,17 @@
       <c r="C26" s="7">
         <v>3</v>
       </c>
-      <c r="E26" s="7">
-        <v>5</v>
-      </c>
-      <c r="G26" s="7">
-        <v>3</v>
-      </c>
-      <c r="I26" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="7">
+        <v>5</v>
+      </c>
+      <c r="H26" s="7">
+        <v>3</v>
+      </c>
+      <c r="J26" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1171,19 +1228,20 @@
         <v>1</v>
       </c>
       <c r="C27"/>
-      <c r="D27">
-        <v>5</v>
-      </c>
-      <c r="E27"/>
+      <c r="D27"/>
+      <c r="E27">
+        <v>5</v>
+      </c>
       <c r="F27"/>
-      <c r="G27">
-        <v>5</v>
-      </c>
-      <c r="I27">
+      <c r="G27"/>
+      <c r="H27">
+        <v>5</v>
+      </c>
+      <c r="J27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>45</v>
       </c>
@@ -1193,23 +1251,23 @@
       <c r="C28" s="7">
         <v>5</v>
       </c>
-      <c r="D28" s="7">
-        <v>4</v>
-      </c>
       <c r="E28" s="7">
-        <v>5</v>
-      </c>
-      <c r="G28" s="7">
-        <v>5</v>
-      </c>
-      <c r="H28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" s="7">
+        <v>5</v>
+      </c>
+      <c r="H28" s="7">
+        <v>5</v>
+      </c>
+      <c r="I28" t="s">
         <v>47</v>
       </c>
-      <c r="I28" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>27</v>
       </c>
@@ -1219,23 +1277,23 @@
       <c r="C29" s="7">
         <v>2</v>
       </c>
-      <c r="D29" s="7">
-        <v>4</v>
-      </c>
       <c r="E29" s="7">
         <v>4</v>
       </c>
-      <c r="G29" s="7">
-        <v>5</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="F29" s="7">
+        <v>4</v>
+      </c>
+      <c r="H29" s="7">
+        <v>5</v>
+      </c>
+      <c r="I29" t="s">
         <v>32</v>
       </c>
-      <c r="I29" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="J29" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -1247,9 +1305,10 @@
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30"/>
-      <c r="I30"/>
-    </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H30"/>
+      <c r="J30"/>
+    </row>
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1261,24 +1320,133 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31"/>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H31"/>
+      <c r="J31"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="7">
+        <v>100000</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>54</v>
+      <c r="C33" s="7">
+        <v>2</v>
+      </c>
+      <c r="D33" s="7">
+        <v>5</v>
+      </c>
+      <c r="F33" s="7">
+        <v>1</v>
+      </c>
+      <c r="H33" s="7">
+        <v>5</v>
+      </c>
+      <c r="I33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="7">
+        <v>2</v>
+      </c>
+      <c r="C34" s="7">
+        <v>5</v>
+      </c>
+      <c r="D34" s="7">
+        <v>5</v>
+      </c>
+      <c r="F34" s="7">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="7">
+        <v>3800</v>
+      </c>
+      <c r="D35" s="7">
+        <v>5</v>
+      </c>
+      <c r="F35" s="7">
+        <v>5</v>
+      </c>
+      <c r="J35" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="7">
+        <v>2</v>
+      </c>
+      <c r="D36" s="7">
+        <v>5</v>
+      </c>
+      <c r="F36" s="7">
+        <v>3</v>
+      </c>
+      <c r="I36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="7">
+        <v>3</v>
+      </c>
+      <c r="D37" s="7">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>3</v>
+      </c>
+      <c r="I37" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="7">
+        <v>3</v>
+      </c>
+      <c r="D38" s="7">
+        <v>5</v>
+      </c>
+      <c r="F38" s="7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I31" xr:uid="{5B8BAF05-1FD3-624C-9941-B290D0C9FED2}">
+  <autoFilter ref="A1:J31" xr:uid="{5B8BAF05-1FD3-624C-9941-B290D0C9FED2}">
     <filterColumn colId="1">
       <filters blank="1">
         <filter val="3"/>
@@ -1286,13 +1454,23 @@
         <filter val="5"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I29">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J29">
       <sortCondition ref="A1:A29"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A1:I1048576">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$I1=1</formula>
+  <conditionalFormatting sqref="A33:A36 C33:J33 D34:J34 A38:B38 A1:J31 A32:C32 E32:J32 A39:J1048576 C35:J36 D38:J38 A37:J37">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$J1=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$J34=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>$J32=1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>